<commit_message>
Removed Reference to fuel consumption
A core change from for the first release is removing the IC only component of fuel consumption. It was further verified that an EV transmission through a single gear with ratio 1.
</commit_message>
<xml_diff>
--- a/OpenVEHICLE tmp.xlsx
+++ b/OpenVEHICLE tmp.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Google Drive\Youtube VD\Release\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3b07fb4c2441c8f0/Documents/GitHub/OpenLAP-Lap-Time-Simulator-EV_Mod/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_88FFB067AC54492510CF52B0C47075E6E28CE6EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{292B3434-63CB-483C-936C-AC0C7543B12F}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8745" windowHeight="12405"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -321,7 +322,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -715,11 +716,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B3" totalsRowShown="0">
-  <autoFilter ref="A1:B3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:B3" totalsRowShown="0">
+  <autoFilter ref="A1:B3" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Engine Speed [rpm]"/>
-    <tableColumn id="2" name="Torque [Nm]"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Engine Speed [rpm]"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Torque [Nm]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -987,22 +988,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C35" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="79.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="79.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="23" t="s">
         <v>44</v>
       </c>
@@ -1019,7 +1020,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="33" t="s">
         <v>0</v>
       </c>
@@ -1032,7 +1033,7 @@
       </c>
       <c r="E2" s="11"/>
     </row>
-    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="34"/>
       <c r="B3" s="12" t="s">
         <v>2</v>
@@ -1043,7 +1044,7 @@
       </c>
       <c r="E3" s="15"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="33" t="s">
         <v>11</v>
       </c>
@@ -1056,7 +1057,7 @@
       </c>
       <c r="E4" s="11"/>
     </row>
-    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="34"/>
       <c r="B5" s="12" t="s">
         <v>4</v>
@@ -1067,7 +1068,7 @@
       </c>
       <c r="E5" s="15"/>
     </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="16" t="s">
         <v>9</v>
       </c>
@@ -1080,7 +1081,7 @@
       </c>
       <c r="E6" s="20"/>
     </row>
-    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="16" t="s">
         <v>10</v>
       </c>
@@ -1095,7 +1096,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="33" t="s">
         <v>13</v>
       </c>
@@ -1110,7 +1111,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="35"/>
       <c r="B9" s="2" t="s">
         <v>72</v>
@@ -1123,7 +1124,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="35"/>
       <c r="B10" s="2" t="s">
         <v>20</v>
@@ -1136,7 +1137,7 @@
       </c>
       <c r="E10" s="21"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="35"/>
       <c r="B11" s="2" t="s">
         <v>21</v>
@@ -1149,7 +1150,7 @@
       </c>
       <c r="E11" s="21"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="35"/>
       <c r="B12" s="2" t="s">
         <v>70</v>
@@ -1160,7 +1161,7 @@
       </c>
       <c r="E12" s="21"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="35"/>
       <c r="B13" s="2" t="s">
         <v>16</v>
@@ -1171,7 +1172,7 @@
       </c>
       <c r="E13" s="21"/>
     </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="34"/>
       <c r="B14" s="12" t="s">
         <v>22</v>
@@ -1184,7 +1185,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="33" t="s">
         <v>19</v>
       </c>
@@ -1199,7 +1200,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="35"/>
       <c r="B16" s="2" t="s">
         <v>24</v>
@@ -1212,7 +1213,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="35"/>
       <c r="B17" s="2" t="s">
         <v>76</v>
@@ -1225,7 +1226,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="35"/>
       <c r="B18" s="2" t="s">
         <v>25</v>
@@ -1238,7 +1239,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="35"/>
       <c r="B19" s="2" t="s">
         <v>26</v>
@@ -1251,7 +1252,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="35"/>
       <c r="B20" s="2" t="s">
         <v>27</v>
@@ -1264,7 +1265,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="34"/>
       <c r="B21" s="12" t="s">
         <v>28</v>
@@ -1277,7 +1278,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="33" t="s">
         <v>29</v>
       </c>
@@ -1292,7 +1293,7 @@
       </c>
       <c r="E22" s="11"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="35"/>
       <c r="B23" s="2" t="s">
         <v>30</v>
@@ -1305,7 +1306,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="35"/>
       <c r="B24" s="2" t="s">
         <v>35</v>
@@ -1318,7 +1319,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="35"/>
       <c r="B25" s="2" t="s">
         <v>31</v>
@@ -1331,7 +1332,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="35"/>
       <c r="B26" s="2" t="s">
         <v>32</v>
@@ -1344,7 +1345,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="35"/>
       <c r="B27" s="2" t="s">
         <v>33</v>
@@ -1357,7 +1358,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="35"/>
       <c r="B28" s="2" t="s">
         <v>38</v>
@@ -1370,7 +1371,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="35"/>
       <c r="B29" s="2" t="s">
         <v>39</v>
@@ -1383,7 +1384,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="35"/>
       <c r="B30" s="2" t="s">
         <v>40</v>
@@ -1396,7 +1397,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="35"/>
       <c r="B31" s="2" t="s">
         <v>41</v>
@@ -1409,7 +1410,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="34"/>
       <c r="B32" s="12" t="s">
         <v>42</v>
@@ -1422,7 +1423,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="33" t="s">
         <v>49</v>
       </c>
@@ -1437,7 +1438,7 @@
       </c>
       <c r="E33" s="11"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="35"/>
       <c r="B34" s="2" t="s">
         <v>51</v>
@@ -1450,7 +1451,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="34"/>
       <c r="B35" s="12" t="s">
         <v>52</v>
@@ -1463,7 +1464,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="30" t="s">
         <v>54</v>
       </c>
@@ -1476,7 +1477,7 @@
       </c>
       <c r="E36" s="11"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="31"/>
       <c r="B37" s="5" t="s">
         <v>77</v>
@@ -1489,12 +1490,14 @@
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="31"/>
       <c r="B38" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C38" s="6"/>
+      <c r="C38" s="6">
+        <v>0.98</v>
+      </c>
       <c r="D38" s="7" t="s">
         <v>37</v>
       </c>
@@ -1502,12 +1505,14 @@
         <v>87</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="31"/>
       <c r="B39" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C39" s="6"/>
+      <c r="C39" s="6">
+        <v>0.98</v>
+      </c>
       <c r="D39" s="7" t="s">
         <v>37</v>
       </c>
@@ -1515,12 +1520,14 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="31"/>
       <c r="B40" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C40" s="6"/>
+      <c r="C40" s="6">
+        <v>1</v>
+      </c>
       <c r="D40" s="7" t="s">
         <v>37</v>
       </c>
@@ -1528,12 +1535,14 @@
         <v>87</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="31"/>
       <c r="B41" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="4"/>
+      <c r="C41" s="4">
+        <v>5</v>
+      </c>
       <c r="D41" s="3" t="s">
         <v>37</v>
       </c>
@@ -1541,122 +1550,144 @@
         <v>96</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="31"/>
       <c r="B42" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C42" s="4"/>
+      <c r="C42" s="4">
+        <v>1</v>
+      </c>
       <c r="D42" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E42" s="21"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="31"/>
       <c r="B43" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="C43" s="4"/>
+      <c r="C43" s="4">
+        <v>1</v>
+      </c>
       <c r="D43" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E43" s="21"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="31"/>
       <c r="B44" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="C44" s="4"/>
+      <c r="C44" s="4">
+        <v>1</v>
+      </c>
       <c r="D44" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E44" s="21"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="31"/>
       <c r="B45" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="C45" s="4"/>
+      <c r="C45" s="4">
+        <v>1</v>
+      </c>
       <c r="D45" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E45" s="21"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="31"/>
       <c r="B46" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="C46" s="4"/>
+      <c r="C46" s="4">
+        <v>1</v>
+      </c>
       <c r="D46" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E46" s="21"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="31"/>
       <c r="B47" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="C47" s="4"/>
+      <c r="C47" s="4">
+        <v>1</v>
+      </c>
       <c r="D47" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E47" s="21"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="31"/>
       <c r="B48" s="27" t="s">
         <v>65</v>
       </c>
-      <c r="C48" s="4"/>
+      <c r="C48" s="4">
+        <v>1</v>
+      </c>
       <c r="D48" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E48" s="21"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="31"/>
       <c r="B49" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="C49" s="4"/>
+      <c r="C49" s="4">
+        <v>1</v>
+      </c>
       <c r="D49" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E49" s="21"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="31"/>
       <c r="B50" s="27" t="s">
         <v>67</v>
       </c>
-      <c r="C50" s="4"/>
+      <c r="C50" s="4">
+        <v>1</v>
+      </c>
       <c r="D50" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E50" s="21"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="31"/>
       <c r="B51" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C51" s="4"/>
+      <c r="C51" s="4">
+        <v>1</v>
+      </c>
       <c r="D51" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E51" s="21"/>
     </row>
-    <row r="52" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="32"/>
       <c r="B52" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="C52" s="13"/>
+      <c r="C52" s="13">
+        <v>1</v>
+      </c>
       <c r="D52" s="14" t="s">
         <v>37</v>
       </c>
@@ -1678,20 +1709,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>14</v>
       </c>
@@ -1699,7 +1730,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1000</v>
       </c>
@@ -1707,7 +1738,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>6000</v>
       </c>

</xml_diff>